<commit_message>
adding quarto template example
</commit_message>
<xml_diff>
--- a/outputs/04 - example - group_x_variable.xlsx
+++ b/outputs/04 - example - group_x_variable.xlsx
@@ -3741,9 +3741,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815AD52C-3AC6-4BE1-A71C-DD89F05C0937}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D441E25-A35F-429F-A1E2-5F345CBB7DA2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F161126C-6A36-4158-BDB2-17072ECC5455}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48879872-C3DD-4F25-8FBB-BD367F707D3A}"/>
 </file>
</xml_diff>